<commit_message>
Modificaciones en campos de BD
✅ Cambiar nombre a los siguientes campos de la DB: usuNombres, usuBoletaAlumnoEgresado, usuNoCelularActual, usuBoletaPosgrado, usuFileNameComprobanteEstudios, usuNoEmpleadoContrato, usuNoExtensionActual, usuCorreoPersonalCuentaActual
✅ Los objetos que se instancian a partir de las Clases DTO/ViewModel Usuario y Solicitudes, se tienen que inicializar los atributos Navigation (ForeigKey) en null
✅ Badge Count Tickets y Lista de Usuarios
</commit_message>
<xml_diff>
--- a/CorreosInstitucionales/Server/wwwroot/assets/sol_alta_desbloqueo.xlsx
+++ b/CorreosInstitucionales/Server/wwwroot/assets/sol_alta_desbloqueo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_alo\Documents\GitHub\CorreosInstitucionales\CorreosInstitucionales\Server\wwwroot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB87AFC-1070-4A9A-A2D8-67612DC5562B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1176A50-B771-4BA5-88B1-94F04BC3F9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,24 +135,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -234,13 +221,10 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,29 +234,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,84 +628,84 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="54.5703125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="45.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="56.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>45408</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="16" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>